<commit_message>
Added Documentation, and some other stats
</commit_message>
<xml_diff>
--- a/Monopoly Datasheet.xlsx
+++ b/Monopoly Datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minja\Documents\GitHub\Monopoly-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31EAB88-990F-4750-A029-3770726FAE81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF16A0E-76A7-446B-88B0-20A21859A406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{D0DAD6BF-A611-478E-A424-5FFB9DDF5D67}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>Mortgage Value is 50%</t>
+  </si>
+  <si>
+    <t>Location</t>
   </si>
 </sst>
 </file>
@@ -592,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF664CEA-D233-468A-B2D2-5C0633FA432F}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -615,30 +618,32 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -651,27 +656,30 @@
         <v>60</v>
       </c>
       <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
         <v>50</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>2</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>10</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>30</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>90</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>160</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>250</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -686,27 +694,30 @@
         <v>60</v>
       </c>
       <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
         <v>50</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>4</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>20</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>60</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>180</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>320</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>450</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -721,27 +732,30 @@
         <v>100</v>
       </c>
       <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
         <v>50</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>6</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>30</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>90</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>270</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>400</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>550</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -756,27 +770,30 @@
         <v>100</v>
       </c>
       <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
         <v>50</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>6</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>30</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>90</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>270</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>400</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>550</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -791,27 +808,30 @@
         <v>120</v>
       </c>
       <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6">
         <v>50</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>8</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>40</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>100</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>300</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>450</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>600</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>33</v>
       </c>
     </row>
@@ -826,27 +846,30 @@
         <v>140</v>
       </c>
       <c r="D7">
+        <v>11</v>
+      </c>
+      <c r="E7">
         <v>100</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>10</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>50</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>150</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>450</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>625</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>750</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>34</v>
       </c>
     </row>
@@ -861,27 +884,30 @@
         <v>140</v>
       </c>
       <c r="D8">
+        <v>13</v>
+      </c>
+      <c r="E8">
         <v>100</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>10</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>50</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>150</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>450</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>625</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>750</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>34</v>
       </c>
     </row>
@@ -896,27 +922,30 @@
         <v>160</v>
       </c>
       <c r="D9">
+        <v>14</v>
+      </c>
+      <c r="E9">
         <v>100</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>12</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>60</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>180</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>500</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>700</v>
       </c>
-      <c r="J9" s="1">
+      <c r="K9" s="1">
         <v>900</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>34</v>
       </c>
     </row>
@@ -931,27 +960,30 @@
         <v>180</v>
       </c>
       <c r="D10">
+        <v>16</v>
+      </c>
+      <c r="E10">
         <v>100</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>14</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>70</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>200</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>550</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>750</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>950</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>35</v>
       </c>
     </row>
@@ -966,27 +998,30 @@
         <v>180</v>
       </c>
       <c r="D11">
+        <v>18</v>
+      </c>
+      <c r="E11">
         <v>100</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>14</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>70</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>200</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>550</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>750</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>950</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1001,27 +1036,30 @@
         <v>200</v>
       </c>
       <c r="D12">
+        <v>19</v>
+      </c>
+      <c r="E12">
         <v>100</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>16</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>80</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>220</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>600</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>800</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>1000</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1036,27 +1074,30 @@
         <v>220</v>
       </c>
       <c r="D13">
+        <v>21</v>
+      </c>
+      <c r="E13">
         <v>150</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>18</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>90</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>250</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>700</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>875</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>1050</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1071,27 +1112,30 @@
         <v>220</v>
       </c>
       <c r="D14">
+        <v>23</v>
+      </c>
+      <c r="E14">
         <v>150</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>18</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>90</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>250</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>700</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>875</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>1050</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1106,27 +1150,30 @@
         <v>240</v>
       </c>
       <c r="D15">
+        <v>24</v>
+      </c>
+      <c r="E15">
         <v>150</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>20</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>100</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>300</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>750</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>925</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>1100</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1141,31 +1188,34 @@
         <v>260</v>
       </c>
       <c r="D16">
+        <v>26</v>
+      </c>
+      <c r="E16">
         <v>150</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>22</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>110</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>330</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>800</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>975</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>1150</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1176,31 +1226,34 @@
         <v>260</v>
       </c>
       <c r="D17">
+        <v>27</v>
+      </c>
+      <c r="E17">
         <v>150</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>22</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>110</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>330</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>800</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>975</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>1150</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1211,31 +1264,34 @@
         <v>280</v>
       </c>
       <c r="D18">
+        <v>29</v>
+      </c>
+      <c r="E18">
         <v>150</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>24</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>120</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>360</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>850</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>1025</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>1200</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1246,31 +1302,34 @@
         <v>300</v>
       </c>
       <c r="D19">
+        <v>31</v>
+      </c>
+      <c r="E19">
         <v>200</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>26</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>130</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>390</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>900</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>1100</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>1275</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1281,31 +1340,34 @@
         <v>300</v>
       </c>
       <c r="D20">
+        <v>32</v>
+      </c>
+      <c r="E20">
         <v>200</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>26</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>130</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>390</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>900</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>1100</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>1275</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1316,31 +1378,34 @@
         <v>320</v>
       </c>
       <c r="D21">
+        <v>34</v>
+      </c>
+      <c r="E21">
         <v>200</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>28</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>150</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>450</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>1000</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>1200</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>1400</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1351,31 +1416,34 @@
         <v>350</v>
       </c>
       <c r="D22">
+        <v>37</v>
+      </c>
+      <c r="E22">
         <v>200</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>35</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>175</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>500</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>1100</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>1300</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>1500</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1386,31 +1454,34 @@
         <v>400</v>
       </c>
       <c r="D23">
+        <v>39</v>
+      </c>
+      <c r="E23">
         <v>200</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>50</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>200</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>600</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>1400</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>1700</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>2000</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1420,20 +1491,23 @@
       <c r="C24">
         <v>200</v>
       </c>
-      <c r="E24">
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="F24">
         <v>25</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>50</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>100</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>200</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1443,20 +1517,23 @@
       <c r="C25">
         <v>200</v>
       </c>
-      <c r="E25">
+      <c r="D25">
+        <v>15</v>
+      </c>
+      <c r="F25">
         <v>25</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>50</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>100</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1466,20 +1543,23 @@
       <c r="C26">
         <v>200</v>
       </c>
-      <c r="E26">
+      <c r="D26">
         <v>25</v>
       </c>
       <c r="F26">
+        <v>25</v>
+      </c>
+      <c r="G26">
         <v>50</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>100</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1489,20 +1569,23 @@
       <c r="C27">
         <v>200</v>
       </c>
-      <c r="E27">
+      <c r="D27">
+        <v>35</v>
+      </c>
+      <c r="F27">
         <v>25</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>50</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>100</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>200</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1512,14 +1595,17 @@
       <c r="C28">
         <v>150</v>
       </c>
-      <c r="E28">
+      <c r="D28">
+        <v>12</v>
+      </c>
+      <c r="F28">
         <v>4</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1529,10 +1615,13 @@
       <c r="C29">
         <v>150</v>
       </c>
-      <c r="E29">
+      <c r="D29">
+        <v>28</v>
+      </c>
+      <c r="F29">
         <v>4</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding more property classes
</commit_message>
<xml_diff>
--- a/Monopoly Datasheet.xlsx
+++ b/Monopoly Datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minja\Documents\GitHub\Monopoly-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF16A0E-76A7-446B-88B0-20A21859A406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9E6683-2A5E-4C05-B75B-E84346D3F109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{D0DAD6BF-A611-478E-A424-5FFB9DDF5D67}"/>
+    <workbookView xWindow="7170" yWindow="10" windowWidth="18430" windowHeight="11170" xr2:uid="{D0DAD6BF-A611-478E-A424-5FFB9DDF5D67}"/>
   </bookViews>
   <sheets>
     <sheet name="Card" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -211,6 +211,12 @@
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>Go</t>
+  </si>
+  <si>
+    <t>Community Chest</t>
   </si>
 </sst>
 </file>
@@ -593,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF664CEA-D233-468A-B2D2-5C0633FA432F}">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1623,6 +1629,25 @@
       </c>
       <c r="G29">
         <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30">
+        <v>200</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>